<commit_message>
CS1_3. Market prices update.
</commit_message>
<xml_diff>
--- a/data/CS1_3/Market Data/CS1_market_data_2020.xlsx
+++ b/data/CS1_3/Market Data/CS1_market_data_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\CS1_3\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FEA2E9-2E36-450B-A19C-37D84B13240B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D1C10B-CB39-484E-A416-2D63AF61B5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -150,12 +150,12 @@
         </row>
         <row r="4">
           <cell r="B4">
-            <v>2.5000000000000001E-2</v>
+            <v>5.0000000000000001E-3</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5">
-            <v>2.5000000000000001E-2</v>
+            <v>5.0000000000000001E-3</v>
           </cell>
         </row>
       </sheetData>
@@ -3456,7 +3456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E73F7F-45E0-423B-A01B-B6DF6F75CAB7}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -4055,7 +4055,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4677,8 +4677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E119D8D-D7FD-46DB-8300-FC3B5CEFAAC8}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>